<commit_message>
add classifier and more test data
</commit_message>
<xml_diff>
--- a/Training_data/670 training data clasification.xlsx
+++ b/Training_data/670 training data clasification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="91">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,18 +298,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -318,7 +318,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,8 +349,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -363,7 +363,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -437,7 +437,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -472,7 +471,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -648,20 +646,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="A1:D230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>301</v>
       </c>
@@ -684,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>301</v>
       </c>
@@ -695,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>301</v>
       </c>
@@ -706,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>301</v>
       </c>
@@ -717,7 +715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>301</v>
       </c>
@@ -728,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>301</v>
       </c>
@@ -739,7 +737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>301</v>
       </c>
@@ -750,7 +748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>301</v>
       </c>
@@ -761,7 +759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>301</v>
       </c>
@@ -772,7 +770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>301</v>
       </c>
@@ -783,7 +781,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>301</v>
       </c>
@@ -794,7 +792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>302</v>
       </c>
@@ -805,7 +803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>302</v>
       </c>
@@ -816,7 +814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>302</v>
       </c>
@@ -827,7 +825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>302</v>
       </c>
@@ -838,7 +836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>302</v>
       </c>
@@ -849,7 +847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>302</v>
       </c>
@@ -860,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>302</v>
       </c>
@@ -871,7 +869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>302</v>
       </c>
@@ -882,7 +880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>302</v>
       </c>
@@ -893,7 +891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>302</v>
       </c>
@@ -904,7 +902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>303</v>
       </c>
@@ -915,7 +913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>303</v>
       </c>
@@ -926,7 +924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>303</v>
       </c>
@@ -937,7 +935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>303</v>
       </c>
@@ -948,7 +946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>303</v>
       </c>
@@ -959,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>304</v>
       </c>
@@ -970,7 +968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>304</v>
       </c>
@@ -981,7 +979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>304</v>
       </c>
@@ -992,7 +990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>304</v>
       </c>
@@ -1003,7 +1001,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>304</v>
       </c>
@@ -1014,7 +1012,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>304</v>
       </c>
@@ -1025,7 +1023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>304</v>
       </c>
@@ -1036,7 +1034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>304</v>
       </c>
@@ -1047,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>304</v>
       </c>
@@ -1058,7 +1056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>305</v>
       </c>
@@ -1069,7 +1067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>305</v>
       </c>
@@ -1080,7 +1078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>305</v>
       </c>
@@ -1091,7 +1089,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>305</v>
       </c>
@@ -1102,7 +1100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>305</v>
       </c>
@@ -1113,7 +1111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>305</v>
       </c>
@@ -1124,7 +1122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>306</v>
       </c>
@@ -1135,7 +1133,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>306</v>
       </c>
@@ -1146,7 +1144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>306</v>
       </c>
@@ -1157,7 +1155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>306</v>
       </c>
@@ -1168,7 +1166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>306</v>
       </c>
@@ -1179,7 +1177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>306</v>
       </c>
@@ -1190,7 +1188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>306</v>
       </c>
@@ -1201,7 +1199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>306</v>
       </c>
@@ -1212,7 +1210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>307</v>
       </c>
@@ -1223,7 +1221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>307</v>
       </c>
@@ -1234,7 +1232,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>307</v>
       </c>
@@ -1245,7 +1243,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>307</v>
       </c>
@@ -1256,7 +1254,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>307</v>
       </c>
@@ -1267,7 +1265,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>307</v>
       </c>
@@ -1278,7 +1276,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>307</v>
       </c>
@@ -1289,7 +1287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>307</v>
       </c>
@@ -1300,7 +1298,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>307</v>
       </c>
@@ -1311,7 +1309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>307</v>
       </c>
@@ -1322,7 +1320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>307</v>
       </c>
@@ -1333,7 +1331,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>307</v>
       </c>
@@ -1344,7 +1342,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>307</v>
       </c>
@@ -1355,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>308</v>
       </c>
@@ -1366,7 +1364,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>308</v>
       </c>
@@ -1377,7 +1375,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>308</v>
       </c>
@@ -1388,7 +1386,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>308</v>
       </c>
@@ -1399,7 +1397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>308</v>
       </c>
@@ -1410,7 +1408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>308</v>
       </c>
@@ -1421,7 +1419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>308</v>
       </c>
@@ -1432,7 +1430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>309</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>309</v>
       </c>
@@ -1454,7 +1452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>309</v>
       </c>
@@ -1465,7 +1463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>309</v>
       </c>
@@ -1476,7 +1474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>309</v>
       </c>
@@ -1487,7 +1485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>310</v>
       </c>
@@ -1498,7 +1496,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>310</v>
       </c>
@@ -1509,7 +1507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>310</v>
       </c>
@@ -1520,7 +1518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>310</v>
       </c>
@@ -1531,7 +1529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>310</v>
       </c>
@@ -1542,7 +1540,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>311</v>
       </c>
@@ -1553,7 +1551,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>311</v>
       </c>
@@ -1564,7 +1562,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>311</v>
       </c>
@@ -1575,7 +1573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>311</v>
       </c>
@@ -1586,7 +1584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>311</v>
       </c>
@@ -1597,7 +1595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>311</v>
       </c>
@@ -1608,7 +1606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>311</v>
       </c>
@@ -1619,7 +1617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>312</v>
       </c>
@@ -1630,7 +1628,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>312</v>
       </c>
@@ -1641,7 +1639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>312</v>
       </c>
@@ -1652,7 +1650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>312</v>
       </c>
@@ -1663,7 +1661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>312</v>
       </c>
@@ -1674,7 +1672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>312</v>
       </c>
@@ -1685,7 +1683,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>312</v>
       </c>
@@ -1696,7 +1694,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>312</v>
       </c>
@@ -1707,7 +1705,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>131</v>
       </c>
@@ -1718,7 +1716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>313</v>
       </c>
@@ -1729,7 +1727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>313</v>
       </c>
@@ -1740,7 +1738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>313</v>
       </c>
@@ -1751,7 +1749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>313</v>
       </c>
@@ -1762,7 +1760,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>313</v>
       </c>
@@ -1773,7 +1771,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:4">
       <c r="A102">
         <v>313</v>
       </c>
@@ -1784,7 +1782,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:4">
       <c r="A103">
         <v>314</v>
       </c>
@@ -1795,7 +1793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:4">
       <c r="A104">
         <v>314</v>
       </c>
@@ -1806,7 +1804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:4">
       <c r="A105">
         <v>314</v>
       </c>
@@ -1817,7 +1815,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:4">
       <c r="A106">
         <v>314</v>
       </c>
@@ -1828,7 +1826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:4">
       <c r="A107">
         <v>314</v>
       </c>
@@ -1839,7 +1837,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:4">
       <c r="A108">
         <v>314</v>
       </c>
@@ -1850,7 +1848,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:4">
       <c r="A109">
         <v>314</v>
       </c>
@@ -1861,7 +1859,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:4">
       <c r="A110">
         <v>315</v>
       </c>
@@ -1872,7 +1870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:4">
       <c r="A111">
         <v>315</v>
       </c>
@@ -1883,7 +1881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:4">
       <c r="A112">
         <v>315</v>
       </c>
@@ -1894,7 +1892,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:4">
       <c r="A113">
         <v>315</v>
       </c>
@@ -1905,7 +1903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:4">
       <c r="A114">
         <v>315</v>
       </c>
@@ -1916,7 +1914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:4">
       <c r="A115">
         <v>315</v>
       </c>
@@ -1927,7 +1925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:4">
       <c r="A116">
         <v>315</v>
       </c>
@@ -1938,7 +1936,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:4">
       <c r="A117">
         <v>315</v>
       </c>
@@ -1949,7 +1947,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:4">
       <c r="A118">
         <v>316</v>
       </c>
@@ -1960,7 +1958,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:4">
       <c r="A119">
         <v>316</v>
       </c>
@@ -1971,7 +1969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:4">
       <c r="A120">
         <v>316</v>
       </c>
@@ -1982,7 +1980,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:4">
       <c r="A121">
         <v>317</v>
       </c>
@@ -1993,7 +1991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:4">
       <c r="A122">
         <v>317</v>
       </c>
@@ -2004,7 +2002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:4">
       <c r="A123">
         <v>317</v>
       </c>
@@ -2015,7 +2013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:4">
       <c r="A124">
         <v>318</v>
       </c>
@@ -2026,7 +2024,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:4">
       <c r="A125">
         <v>318</v>
       </c>
@@ -2037,7 +2035,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:4">
       <c r="A126">
         <v>318</v>
       </c>
@@ -2048,7 +2046,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:4">
       <c r="A127">
         <v>318</v>
       </c>
@@ -2059,7 +2057,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:4">
       <c r="A128">
         <v>318</v>
       </c>
@@ -2070,7 +2068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:4">
       <c r="A129">
         <v>318</v>
       </c>
@@ -2081,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:4">
       <c r="A130">
         <v>319</v>
       </c>
@@ -2092,7 +2090,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:4">
       <c r="A131">
         <v>319</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:4">
       <c r="A132">
         <v>319</v>
       </c>
@@ -2114,7 +2112,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:4">
       <c r="A133">
         <v>319</v>
       </c>
@@ -2125,7 +2123,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:4">
       <c r="A134">
         <v>319</v>
       </c>
@@ -2136,7 +2134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:4">
       <c r="A135">
         <v>319</v>
       </c>
@@ -2147,7 +2145,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:4">
       <c r="A136">
         <v>320</v>
       </c>
@@ -2158,7 +2156,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:4">
       <c r="A137">
         <v>320</v>
       </c>
@@ -2169,7 +2167,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:4">
       <c r="A138">
         <v>320</v>
       </c>
@@ -2180,7 +2178,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:4">
       <c r="A139">
         <v>320</v>
       </c>
@@ -2191,7 +2189,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:4">
       <c r="A140">
         <v>320</v>
       </c>
@@ -2202,7 +2200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:4">
       <c r="A141">
         <v>320</v>
       </c>
@@ -2213,7 +2211,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:4">
       <c r="A142">
         <v>320</v>
       </c>
@@ -2224,7 +2222,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:4">
       <c r="A143">
         <v>320</v>
       </c>
@@ -2235,7 +2233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:4">
       <c r="A144">
         <v>320</v>
       </c>
@@ -2246,7 +2244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4">
       <c r="A145">
         <v>320</v>
       </c>
@@ -2257,7 +2255,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4">
       <c r="A146">
         <v>321</v>
       </c>
@@ -2268,7 +2266,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>321</v>
       </c>
@@ -2279,7 +2277,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:4">
       <c r="A148">
         <v>321</v>
       </c>
@@ -2290,7 +2288,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:4">
       <c r="A149">
         <v>321</v>
       </c>
@@ -2301,7 +2299,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:4">
       <c r="A150">
         <v>321</v>
       </c>
@@ -2312,7 +2310,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:4">
       <c r="A151">
         <v>321</v>
       </c>
@@ -2323,7 +2321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:4">
       <c r="A152">
         <v>321</v>
       </c>
@@ -2334,7 +2332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:4">
       <c r="A153">
         <v>321</v>
       </c>
@@ -2345,7 +2343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:4">
       <c r="A154">
         <v>321</v>
       </c>
@@ -2356,7 +2354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:4">
       <c r="A155">
         <v>321</v>
       </c>
@@ -2367,7 +2365,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:4">
       <c r="A156">
         <v>322</v>
       </c>
@@ -2378,7 +2376,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:4">
       <c r="A157">
         <v>322</v>
       </c>
@@ -2389,7 +2387,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:4">
       <c r="A158">
         <v>322</v>
       </c>
@@ -2400,7 +2398,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:4">
       <c r="A159">
         <v>322</v>
       </c>
@@ -2411,7 +2409,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:4">
       <c r="A160">
         <v>322</v>
       </c>
@@ -2422,7 +2420,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:4">
       <c r="A161">
         <v>322</v>
       </c>
@@ -2433,7 +2431,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:4">
       <c r="A162">
         <v>322</v>
       </c>
@@ -2444,7 +2442,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:4">
       <c r="A163">
         <v>322</v>
       </c>
@@ -2455,7 +2453,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:4">
       <c r="A164">
         <v>322</v>
       </c>
@@ -2466,7 +2464,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:4">
       <c r="A165">
         <v>322</v>
       </c>
@@ -2477,7 +2475,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:4">
       <c r="A166">
         <v>322</v>
       </c>
@@ -2488,7 +2486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:4">
       <c r="A167">
         <v>322</v>
       </c>
@@ -2499,7 +2497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:4">
       <c r="A168">
         <v>322</v>
       </c>
@@ -2510,7 +2508,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:4">
       <c r="A169">
         <v>322</v>
       </c>
@@ -2521,7 +2519,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:4">
       <c r="A170">
         <v>323</v>
       </c>
@@ -2532,7 +2530,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:4">
       <c r="A171">
         <v>323</v>
       </c>
@@ -2543,7 +2541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:4">
       <c r="A172">
         <v>323</v>
       </c>
@@ -2554,7 +2552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:4">
       <c r="A173">
         <v>323</v>
       </c>
@@ -2565,7 +2563,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:4">
       <c r="A174">
         <v>323</v>
       </c>
@@ -2576,7 +2574,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:4">
       <c r="A175">
         <v>323</v>
       </c>
@@ -2587,7 +2585,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:4">
       <c r="A176">
         <v>323</v>
       </c>
@@ -2598,7 +2596,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:4">
       <c r="A177">
         <v>324</v>
       </c>
@@ -2609,7 +2607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:4">
       <c r="A178">
         <v>324</v>
       </c>
@@ -2620,7 +2618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:4">
       <c r="A179">
         <v>324</v>
       </c>
@@ -2631,7 +2629,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:4">
       <c r="A180">
         <v>324</v>
       </c>
@@ -2642,7 +2640,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:4">
       <c r="A181">
         <v>324</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:4">
       <c r="A182">
         <v>325</v>
       </c>
@@ -2664,7 +2662,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:4">
       <c r="A183">
         <v>325</v>
       </c>
@@ -2675,7 +2673,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:4">
       <c r="A184">
         <v>325</v>
       </c>
@@ -2686,7 +2684,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:4">
       <c r="A185">
         <v>325</v>
       </c>
@@ -2697,7 +2695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:4">
       <c r="A186">
         <v>325</v>
       </c>
@@ -2708,7 +2706,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:4">
       <c r="A187">
         <v>325</v>
       </c>
@@ -2719,7 +2717,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:4">
       <c r="A188">
         <v>325</v>
       </c>
@@ -2730,7 +2728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:4">
       <c r="A189">
         <v>325</v>
       </c>
@@ -2741,7 +2739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:4">
       <c r="A190">
         <v>325</v>
       </c>
@@ -2752,7 +2750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:4">
       <c r="A191">
         <v>325</v>
       </c>
@@ -2763,7 +2761,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:4">
       <c r="A192">
         <v>326</v>
       </c>
@@ -2774,7 +2772,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:4">
       <c r="A193">
         <v>326</v>
       </c>
@@ -2785,7 +2783,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:4">
       <c r="A194">
         <v>326</v>
       </c>
@@ -2796,7 +2794,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:4">
       <c r="A195">
         <v>326</v>
       </c>
@@ -2807,7 +2805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:4">
       <c r="A196">
         <v>326</v>
       </c>
@@ -2818,7 +2816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:4">
       <c r="A197">
         <v>326</v>
       </c>
@@ -2829,7 +2827,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:4">
       <c r="A198">
         <v>326</v>
       </c>
@@ -2840,7 +2838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:4">
       <c r="A199">
         <v>327</v>
       </c>
@@ -2851,7 +2849,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:4">
       <c r="A200">
         <v>327</v>
       </c>
@@ -2862,7 +2860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:4">
       <c r="A201">
         <v>327</v>
       </c>
@@ -2873,7 +2871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:4">
       <c r="A202">
         <v>327</v>
       </c>
@@ -2884,7 +2882,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:4">
       <c r="A203">
         <v>327</v>
       </c>
@@ -2895,7 +2893,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:4">
       <c r="A204">
         <v>328</v>
       </c>
@@ -2906,7 +2904,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:4">
       <c r="A205">
         <v>328</v>
       </c>
@@ -2917,7 +2915,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:4">
       <c r="A206">
         <v>328</v>
       </c>
@@ -2928,7 +2926,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:4">
       <c r="A207">
         <v>328</v>
       </c>
@@ -2939,7 +2937,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:4">
       <c r="A208">
         <v>328</v>
       </c>
@@ -2950,7 +2948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:4">
       <c r="A209">
         <v>328</v>
       </c>
@@ -2961,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:4">
       <c r="A210">
         <v>328</v>
       </c>
@@ -2972,7 +2970,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:4">
       <c r="A211">
         <v>328</v>
       </c>
@@ -2983,7 +2981,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:4">
       <c r="A212">
         <v>329</v>
       </c>
@@ -2994,7 +2992,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:4">
       <c r="A213">
         <v>329</v>
       </c>
@@ -3005,7 +3003,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:4">
       <c r="A214">
         <v>329</v>
       </c>
@@ -3016,7 +3014,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:4">
       <c r="A215">
         <v>329</v>
       </c>
@@ -3027,7 +3025,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:4">
       <c r="A216">
         <v>329</v>
       </c>
@@ -3038,7 +3036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:4">
       <c r="A217">
         <v>329</v>
       </c>
@@ -3049,7 +3047,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:4">
       <c r="A218">
         <v>329</v>
       </c>
@@ -3060,7 +3058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:4">
       <c r="A219">
         <v>329</v>
       </c>
@@ -3071,7 +3069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:4">
       <c r="A220">
         <v>329</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:4">
       <c r="A221">
         <v>329</v>
       </c>
@@ -3093,7 +3091,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:4">
       <c r="A222">
         <v>330</v>
       </c>
@@ -3104,7 +3102,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:4">
       <c r="A223">
         <v>330</v>
       </c>
@@ -3115,7 +3113,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:4">
       <c r="A224">
         <v>330</v>
       </c>
@@ -3126,7 +3124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:4">
       <c r="A225">
         <v>330</v>
       </c>
@@ -3137,7 +3135,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:4">
       <c r="A226">
         <v>330</v>
       </c>
@@ -3148,7 +3146,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:4">
       <c r="A227">
         <v>331</v>
       </c>
@@ -3159,7 +3157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:4">
       <c r="A228">
         <v>331</v>
       </c>
@@ -3170,7 +3168,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:4">
       <c r="A229">
         <v>331</v>
       </c>
@@ -3181,7 +3179,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:4">
       <c r="A230">
         <v>331</v>
       </c>
@@ -3431,16 +3429,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>301</v>
       </c>
@@ -3451,7 +3449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>302</v>
       </c>
@@ -3462,7 +3460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>302</v>
       </c>
@@ -3473,7 +3471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>302</v>
       </c>
@@ -3484,7 +3482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>304</v>
       </c>
@@ -3495,7 +3493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>304</v>
       </c>
@@ -3506,7 +3504,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>304</v>
       </c>
@@ -3517,7 +3515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>306</v>
       </c>
@@ -3528,7 +3526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>306</v>
       </c>
@@ -3539,7 +3537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>306</v>
       </c>
@@ -3550,7 +3548,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>307</v>
       </c>
@@ -3561,7 +3559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>307</v>
       </c>
@@ -3572,7 +3570,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>307</v>
       </c>
@@ -3583,7 +3581,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>308</v>
       </c>
@@ -3594,7 +3592,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>308</v>
       </c>
@@ -3605,7 +3603,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>312</v>
       </c>
@@ -3616,7 +3614,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>318</v>
       </c>
@@ -3627,7 +3625,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>318</v>
       </c>
@@ -3638,7 +3636,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>318</v>
       </c>
@@ -3649,7 +3647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>319</v>
       </c>
@@ -3660,7 +3658,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>319</v>
       </c>
@@ -3671,7 +3669,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>320</v>
       </c>
@@ -3682,7 +3680,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>320</v>
       </c>
@@ -3693,7 +3691,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>320</v>
       </c>
@@ -3704,7 +3702,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>321</v>
       </c>
@@ -3715,7 +3713,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>321</v>
       </c>
@@ -3726,7 +3724,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>321</v>
       </c>
@@ -3737,7 +3735,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>322</v>
       </c>
@@ -3748,7 +3746,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>322</v>
       </c>
@@ -3759,7 +3757,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>322</v>
       </c>
@@ -3770,7 +3768,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>322</v>
       </c>
@@ -3781,7 +3779,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>322</v>
       </c>
@@ -3792,7 +3790,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>325</v>
       </c>
@@ -3803,7 +3801,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>325</v>
       </c>
@@ -3814,7 +3812,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>325</v>
       </c>
@@ -3825,7 +3823,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>328</v>
       </c>
@@ -3836,7 +3834,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>328</v>
       </c>
@@ -3893,16 +3891,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D230"/>
   <sheetViews>
     <sheetView topLeftCell="A193" workbookViewId="0">
       <selection activeCell="A207" sqref="A207:XFD207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3913,26 +3911,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>301</v>
       </c>
@@ -3943,19 +3941,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>302</v>
       </c>
@@ -3966,10 +3964,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>302</v>
       </c>
@@ -3980,7 +3978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>302</v>
       </c>
@@ -3991,40 +3989,40 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>304</v>
       </c>
@@ -4035,7 +4033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>304</v>
       </c>
@@ -4046,10 +4044,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>304</v>
       </c>
@@ -4060,43 +4058,43 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>306</v>
       </c>
@@ -4107,7 +4105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>306</v>
       </c>
@@ -4118,7 +4116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>306</v>
       </c>
@@ -4129,22 +4127,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>307</v>
       </c>
@@ -4155,10 +4153,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>307</v>
       </c>
@@ -4169,7 +4167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>307</v>
       </c>
@@ -4180,10 +4178,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>307</v>
       </c>
@@ -4194,10 +4192,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>307</v>
       </c>
@@ -4208,22 +4206,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>308</v>
       </c>
@@ -4234,7 +4232,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>308</v>
       </c>
@@ -4245,70 +4243,70 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4">
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4">
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4">
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4">
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4">
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4">
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4">
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4">
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4">
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4">
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4">
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4">
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4">
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:4">
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:4">
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:4">
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:4">
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>312</v>
       </c>
@@ -4319,115 +4317,115 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:4">
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:4">
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:4">
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:4">
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:4">
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:4">
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:4">
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:4">
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="97" spans="4:4">
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="98" spans="4:4">
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="99" spans="4:4">
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="100" spans="4:4">
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="101" spans="4:4">
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="102" spans="4:4">
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="103" spans="4:4">
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="104" spans="4:4">
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="105" spans="4:4">
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="106" spans="4:4">
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="107" spans="4:4">
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="108" spans="4:4">
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="109" spans="4:4">
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="110" spans="4:4">
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="111" spans="4:4">
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="112" spans="4:4">
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:4">
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:4">
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:4">
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:4">
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:4">
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:4">
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:4">
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:4">
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:4">
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:4">
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:4">
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:4">
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:4">
       <c r="A125">
         <v>318</v>
       </c>
@@ -4438,7 +4436,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:4">
       <c r="A126">
         <v>318</v>
       </c>
@@ -4449,7 +4447,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:4">
       <c r="A127">
         <v>318</v>
       </c>
@@ -4460,13 +4458,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:4">
       <c r="D128" s="1"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:4">
       <c r="D129" s="1"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:4">
       <c r="A130">
         <v>319</v>
       </c>
@@ -4477,10 +4475,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:4">
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:4">
       <c r="A132">
         <v>319</v>
       </c>
@@ -4491,16 +4489,16 @@
         <v>53</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:4">
       <c r="D133" s="1"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:4">
       <c r="D134" s="1"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:4">
       <c r="D135" s="1"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:4">
       <c r="A136">
         <v>320</v>
       </c>
@@ -4511,7 +4509,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:4">
       <c r="A137">
         <v>320</v>
       </c>
@@ -4522,7 +4520,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:4">
       <c r="A138">
         <v>320</v>
       </c>
@@ -4533,7 +4531,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:4">
       <c r="A139">
         <v>320</v>
       </c>
@@ -4544,28 +4542,28 @@
         <v>57</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:4">
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:4">
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:4">
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:4">
       <c r="D143" s="1"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:4">
       <c r="D144" s="1"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4">
       <c r="D145" s="1"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4">
       <c r="D146" s="1"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>321</v>
       </c>
@@ -4576,7 +4574,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:4">
       <c r="A148">
         <v>321</v>
       </c>
@@ -4587,10 +4585,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:4">
       <c r="D149" s="1"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:4">
       <c r="A150">
         <v>321</v>
       </c>
@@ -4601,28 +4599,28 @@
         <v>56</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:4">
       <c r="D151" s="1"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:4">
       <c r="D152" s="1"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:4">
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:4">
       <c r="D154" s="1"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:4">
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:4">
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:4">
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:4">
       <c r="A158">
         <v>322</v>
       </c>
@@ -4633,7 +4631,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:4">
       <c r="A159">
         <v>322</v>
       </c>
@@ -4644,7 +4642,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:4">
       <c r="A160">
         <v>322</v>
       </c>
@@ -4655,7 +4653,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:4">
       <c r="A161">
         <v>322</v>
       </c>
@@ -4666,10 +4664,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:4">
       <c r="D162" s="1"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:4">
       <c r="A163">
         <v>322</v>
       </c>
@@ -4680,61 +4678,61 @@
         <v>56</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:4">
       <c r="D164" s="1"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:4">
       <c r="D165" s="1"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:4">
       <c r="D166" s="1"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:4">
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:4">
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:4">
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:4">
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:4">
       <c r="D171" s="1"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:4">
       <c r="D172" s="1"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:4">
       <c r="D173" s="1"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:4">
       <c r="D174" s="1"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:4">
       <c r="D175" s="1"/>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:4">
       <c r="D176" s="1"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:4">
       <c r="D177" s="1"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:4">
       <c r="D178" s="1"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:4">
       <c r="D179" s="1"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:4">
       <c r="D180" s="1"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:4">
       <c r="D181" s="1"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:4">
       <c r="A182">
         <v>325</v>
       </c>
@@ -4745,7 +4743,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:4">
       <c r="A183">
         <v>325</v>
       </c>
@@ -4756,16 +4754,16 @@
         <v>74</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:4">
       <c r="D184" s="1"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:4">
       <c r="D185" s="1"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:4">
       <c r="D186" s="1"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:4">
       <c r="A187">
         <v>325</v>
       </c>
@@ -4776,58 +4774,58 @@
         <v>77</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:4">
       <c r="D188" s="1"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:4">
       <c r="D189" s="1"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:4">
       <c r="D190" s="1"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:4">
       <c r="D191" s="1"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:4">
       <c r="D192" s="1"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:4">
       <c r="D193" s="1"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:4">
       <c r="D194" s="1"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:4">
       <c r="D195" s="1"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:4">
       <c r="D196" s="1"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:4">
       <c r="D197" s="1"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:4">
       <c r="D198" s="1"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:4">
       <c r="D199" s="1"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:4">
       <c r="D200" s="1"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:4">
       <c r="D201" s="1"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:4">
       <c r="D202" s="1"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:4">
       <c r="D203" s="1"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:4">
       <c r="D204" s="1"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:4">
       <c r="A205">
         <v>328</v>
       </c>
@@ -4838,10 +4836,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:4">
       <c r="D206" s="1"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:4">
       <c r="A207">
         <v>328</v>
       </c>
@@ -4852,73 +4850,73 @@
         <v>85</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:4">
       <c r="D208" s="1"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="209" spans="4:4">
       <c r="D209" s="1"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="210" spans="4:4">
       <c r="D210" s="1"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="211" spans="4:4">
       <c r="D211" s="1"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="212" spans="4:4">
       <c r="D212" s="1"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="213" spans="4:4">
       <c r="D213" s="1"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="214" spans="4:4">
       <c r="D214" s="1"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="215" spans="4:4">
       <c r="D215" s="1"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="216" spans="4:4">
       <c r="D216" s="1"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="217" spans="4:4">
       <c r="D217" s="1"/>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="218" spans="4:4">
       <c r="D218" s="1"/>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="219" spans="4:4">
       <c r="D219" s="1"/>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="220" spans="4:4">
       <c r="D220" s="1"/>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="221" spans="4:4">
       <c r="D221" s="1"/>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="222" spans="4:4">
       <c r="D222" s="1"/>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="223" spans="4:4">
       <c r="D223" s="1"/>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="224" spans="4:4">
       <c r="D224" s="1"/>
     </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="225" spans="4:4">
       <c r="D225" s="1"/>
     </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="226" spans="4:4">
       <c r="D226" s="1"/>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="227" spans="4:4">
       <c r="D227" s="1"/>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="228" spans="4:4">
       <c r="D228" s="1"/>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="229" spans="4:4">
       <c r="D229" s="1"/>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.15">
+    <row r="230" spans="4:4">
       <c r="D230" s="1"/>
     </row>
   </sheetData>
@@ -4970,16 +4968,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>301</v>
       </c>
@@ -4990,7 +4988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>302</v>
       </c>
@@ -4998,32 +4996,32 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>302</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>304</v>
       </c>
@@ -5031,43 +5029,43 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>304</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>306</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>306</v>
       </c>
@@ -5075,109 +5073,109 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>307</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>307</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>307</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>307</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>308</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>318</v>
       </c>
@@ -5185,32 +5183,32 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>318</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>319</v>
       </c>
@@ -5218,120 +5216,120 @@
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>320</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>320</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>320</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>321</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>321</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>322</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>322</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>322</v>
       </c>
@@ -5339,32 +5337,32 @@
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>322</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>325</v>
       </c>
@@ -5372,50 +5370,39 @@
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>325</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>328</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40">
-        <v>328</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="D40" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5423,47 +5410,46 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=01&amp;eventdatetime_id=11372&amp;"/>
-    <hyperlink ref="D2" r:id="rId2" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=02&amp;eventdatetime_id=14194&amp;"/>
-    <hyperlink ref="D3" r:id="rId3" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=02&amp;eventdatetime_id=13408&amp;"/>
-    <hyperlink ref="D4" r:id="rId4" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=02&amp;eventdatetime_id=11373&amp;"/>
-    <hyperlink ref="D5" r:id="rId5" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=04&amp;eventdatetime_id=14478&amp;"/>
-    <hyperlink ref="D6" r:id="rId6" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=04&amp;eventdatetime_id=14373&amp;"/>
-    <hyperlink ref="D7" r:id="rId7" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=04&amp;eventdatetime_id=14992&amp;"/>
-    <hyperlink ref="D8" r:id="rId8" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=06&amp;eventdatetime_id=14493&amp;"/>
-    <hyperlink ref="D9" r:id="rId9" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=06&amp;eventdatetime_id=14043&amp;"/>
-    <hyperlink ref="D10" r:id="rId10" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=06&amp;eventdatetime_id=15099&amp;"/>
-    <hyperlink ref="D11" r:id="rId11" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=14995&amp;"/>
-    <hyperlink ref="D12" r:id="rId12" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=14623&amp;"/>
-    <hyperlink ref="D13" r:id="rId13" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=14827&amp;"/>
-    <hyperlink ref="D14" r:id="rId14" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=12257&amp;"/>
-    <hyperlink ref="D15" r:id="rId15" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=12594&amp;"/>
-    <hyperlink ref="D16" r:id="rId16" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=08&amp;eventdatetime_id=14656&amp;"/>
-    <hyperlink ref="D17" r:id="rId17" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=08&amp;eventdatetime_id=15079&amp;"/>
-    <hyperlink ref="D18" r:id="rId18" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=12&amp;eventdatetime_id=12300&amp;"/>
-    <hyperlink ref="D19" r:id="rId19" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=18&amp;eventdatetime_id=14374&amp;"/>
-    <hyperlink ref="D20" r:id="rId20" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=18&amp;eventdatetime_id=15090&amp;"/>
-    <hyperlink ref="D21" r:id="rId21" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=18&amp;eventdatetime_id=15036&amp;"/>
-    <hyperlink ref="D22" r:id="rId22" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=19&amp;eventdatetime_id=12289&amp;"/>
-    <hyperlink ref="D23" r:id="rId23" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=19&amp;eventdatetime_id=15081&amp;"/>
-    <hyperlink ref="D24" r:id="rId24" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=14074&amp;"/>
-    <hyperlink ref="D25" r:id="rId25" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=14562&amp;"/>
-    <hyperlink ref="D26" r:id="rId26" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=11380&amp;"/>
-    <hyperlink ref="D27" r:id="rId27" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=14075&amp;"/>
-    <hyperlink ref="D28" r:id="rId28" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=21&amp;eventdatetime_id=12281&amp;"/>
-    <hyperlink ref="D29" r:id="rId29" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=21&amp;eventdatetime_id=14985&amp;"/>
-    <hyperlink ref="D30" r:id="rId30" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=21&amp;eventdatetime_id=11381&amp;"/>
-    <hyperlink ref="D31" r:id="rId31" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=14232&amp;"/>
-    <hyperlink ref="D32" r:id="rId32" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=14442&amp;"/>
-    <hyperlink ref="D33" r:id="rId33" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=14244&amp;"/>
-    <hyperlink ref="D34" r:id="rId34" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=12470&amp;"/>
-    <hyperlink ref="D35" r:id="rId35" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=11382&amp;"/>
-    <hyperlink ref="D36" r:id="rId36" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=25&amp;eventdatetime_id=14375&amp;"/>
-    <hyperlink ref="D37" r:id="rId37" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=25&amp;eventdatetime_id=15211&amp;"/>
-    <hyperlink ref="D38" r:id="rId38" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=25&amp;eventdatetime_id=15118&amp;"/>
-    <hyperlink ref="D39" r:id="rId39" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=28&amp;eventdatetime_id=13912&amp;"/>
-    <hyperlink ref="D40" r:id="rId40" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=28&amp;eventdatetime_id=15155&amp;"/>
+    <hyperlink ref="D2" r:id="rId2" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=02&amp;eventdatetime_id=13408&amp;"/>
+    <hyperlink ref="D3" r:id="rId3" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=02&amp;eventdatetime_id=11373&amp;"/>
+    <hyperlink ref="D4" r:id="rId4" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=04&amp;eventdatetime_id=14478&amp;"/>
+    <hyperlink ref="D5" r:id="rId5" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=04&amp;eventdatetime_id=14373&amp;"/>
+    <hyperlink ref="D6" r:id="rId6" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=04&amp;eventdatetime_id=14992&amp;"/>
+    <hyperlink ref="D7" r:id="rId7" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=06&amp;eventdatetime_id=14493&amp;"/>
+    <hyperlink ref="D8" r:id="rId8" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=06&amp;eventdatetime_id=14043&amp;"/>
+    <hyperlink ref="D9" r:id="rId9" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=06&amp;eventdatetime_id=15099&amp;"/>
+    <hyperlink ref="D10" r:id="rId10" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=14995&amp;"/>
+    <hyperlink ref="D11" r:id="rId11" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=14623&amp;"/>
+    <hyperlink ref="D12" r:id="rId12" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=14827&amp;"/>
+    <hyperlink ref="D13" r:id="rId13" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=12257&amp;"/>
+    <hyperlink ref="D14" r:id="rId14" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=07&amp;eventdatetime_id=12594&amp;"/>
+    <hyperlink ref="D15" r:id="rId15" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=08&amp;eventdatetime_id=14656&amp;"/>
+    <hyperlink ref="D16" r:id="rId16" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=08&amp;eventdatetime_id=15079&amp;"/>
+    <hyperlink ref="D17" r:id="rId17" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=12&amp;eventdatetime_id=12300&amp;"/>
+    <hyperlink ref="D18" r:id="rId18" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=18&amp;eventdatetime_id=14374&amp;"/>
+    <hyperlink ref="D19" r:id="rId19" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=18&amp;eventdatetime_id=15090&amp;"/>
+    <hyperlink ref="D20" r:id="rId20" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=18&amp;eventdatetime_id=15036&amp;"/>
+    <hyperlink ref="D21" r:id="rId21" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=19&amp;eventdatetime_id=12289&amp;"/>
+    <hyperlink ref="D22" r:id="rId22" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=19&amp;eventdatetime_id=15081&amp;"/>
+    <hyperlink ref="D23" r:id="rId23" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=14074&amp;"/>
+    <hyperlink ref="D24" r:id="rId24" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=14562&amp;"/>
+    <hyperlink ref="D25" r:id="rId25" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=11380&amp;"/>
+    <hyperlink ref="D26" r:id="rId26" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=20&amp;eventdatetime_id=14075&amp;"/>
+    <hyperlink ref="D27" r:id="rId27" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=21&amp;eventdatetime_id=12281&amp;"/>
+    <hyperlink ref="D28" r:id="rId28" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=21&amp;eventdatetime_id=14985&amp;"/>
+    <hyperlink ref="D29" r:id="rId29" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=21&amp;eventdatetime_id=11381&amp;"/>
+    <hyperlink ref="D30" r:id="rId30" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=14232&amp;"/>
+    <hyperlink ref="D31" r:id="rId31" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=14442&amp;"/>
+    <hyperlink ref="D32" r:id="rId32" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=14244&amp;"/>
+    <hyperlink ref="D33" r:id="rId33" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=12470&amp;"/>
+    <hyperlink ref="D34" r:id="rId34" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=22&amp;eventdatetime_id=11382&amp;"/>
+    <hyperlink ref="D35" r:id="rId35" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=25&amp;eventdatetime_id=14375&amp;"/>
+    <hyperlink ref="D36" r:id="rId36" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=25&amp;eventdatetime_id=15211&amp;"/>
+    <hyperlink ref="D37" r:id="rId37" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=25&amp;eventdatetime_id=15118&amp;"/>
+    <hyperlink ref="D38" r:id="rId38" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=28&amp;eventdatetime_id=13912&amp;"/>
+    <hyperlink ref="D39" r:id="rId39" display="http://calendar.tamu.edu/?&amp;y=2013&amp;m=03&amp;d=28&amp;eventdatetime_id=15155&amp;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId41"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>